<commit_message>
A user just can receive one invitation by day and year almost ok
</commit_message>
<xml_diff>
--- a/uploads/usersmareta.xlsx
+++ b/uploads/usersmareta.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Table 1</t>
   </si>
@@ -42,21 +42,6 @@
   </si>
   <si>
     <t>davichon1985@hotmail.com</t>
-  </si>
-  <si>
-    <t>Pacofiestas</t>
-  </si>
-  <si>
-    <t>12-04-1990</t>
-  </si>
-  <si>
-    <t>luismax@gmail.com</t>
-  </si>
-  <si>
-    <t>cliente</t>
-  </si>
-  <si>
-    <t>randomemail@email.com</t>
   </si>
 </sst>
 </file>
@@ -307,7 +292,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="E6" activeCellId="0" sqref="E6"/>
+      <selection pane="bottomRight" activeCell="C6" activeCellId="0" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18"/>
@@ -381,15 +366,9 @@
       <c r="I4" s="4"/>
     </row>
     <row r="5" customFormat="false" ht="20.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>11</v>
-      </c>
+      <c r="A5" s="7"/>
+      <c r="B5" s="4"/>
+      <c r="C5" s="5"/>
       <c r="D5" s="4"/>
       <c r="E5" s="4"/>
       <c r="F5" s="4"/>
@@ -398,15 +377,9 @@
       <c r="I5" s="4"/>
     </row>
     <row r="6" customFormat="false" ht="20.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>13</v>
-      </c>
+      <c r="A6" s="3"/>
+      <c r="B6" s="4"/>
+      <c r="C6" s="5"/>
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
       <c r="F6" s="4"/>
@@ -608,8 +581,6 @@
   <hyperlinks>
     <hyperlink ref="C3" r:id="rId1" display="daviddsrperiodismo@gmail.com"/>
     <hyperlink ref="C4" r:id="rId2" display="davichon1985@hotmail.com"/>
-    <hyperlink ref="C5" r:id="rId3" display="luismax@gmail.com"/>
-    <hyperlink ref="C6" r:id="rId4" display="randomemail@email.com"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.5"/>

</xml_diff>

<commit_message>
A user cannot receive 2 invitations the same day finally works
</commit_message>
<xml_diff>
--- a/uploads/usersmareta.xlsx
+++ b/uploads/usersmareta.xlsx
@@ -32,7 +32,7 @@
     <t>david</t>
   </si>
   <si>
-    <t>12-04-2022</t>
+    <t>14-04-2022</t>
   </si>
   <si>
     <t>daviddsrperiodismo@gmail.com</t>
@@ -292,7 +292,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="C6" activeCellId="0" sqref="C6"/>
+      <selection pane="bottomRight" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18"/>
@@ -353,7 +353,7 @@
         <v>7</v>
       </c>
       <c r="B4" s="6" t="n">
-        <v>170670</v>
+        <v>170672</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>8</v>

</xml_diff>